<commit_message>
Realizada rota para busca das publicações
</commit_message>
<xml_diff>
--- a/docs/Requisitos_Funcionais.xlsx
+++ b/docs/Requisitos_Funcionais.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oryc1\Desktop\FORUM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desenvolvimento\Desktop\FORUM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483807E8-FF2B-4AED-8491-BEE5D382BE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE91E58-78FF-46D6-A4A7-41CCB2F2B98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{40153BD5-6B4E-464B-9827-E0D7A3498535}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40153BD5-6B4E-464B-9827-E0D7A3498535}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>Tela de cadastro</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>PROJETO FÓRUM DOLCE AMORE</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -519,13 +522,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -537,13 +549,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -860,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3AC791-6796-4544-B0F5-EEDA6635AEE9}">
-  <dimension ref="B1:E26"/>
+  <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,30 +879,30 @@
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
@@ -905,8 +911,11 @@
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -920,7 +929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
@@ -934,7 +943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
@@ -946,7 +955,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
@@ -959,8 +968,11 @@
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
@@ -973,8 +985,11 @@
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
@@ -987,8 +1002,11 @@
       <c r="E10" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1001,8 +1019,11 @@
       <c r="E11" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
@@ -1015,8 +1036,11 @@
       <c r="E12" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
@@ -1026,7 +1050,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1040,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>38</v>
       </c>
@@ -1054,7 +1078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
@@ -1067,8 +1091,11 @@
       <c r="E16" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>49</v>
       </c>
@@ -1081,8 +1108,11 @@
       <c r="E17" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
@@ -1095,8 +1125,11 @@
       <c r="E18" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>51</v>
       </c>
@@ -1109,8 +1142,11 @@
       <c r="E19" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>48</v>
       </c>
@@ -1124,7 +1160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>52</v>
       </c>
@@ -1138,7 +1174,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
@@ -1152,7 +1188,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>58</v>
       </c>
@@ -1166,7 +1202,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>61</v>
       </c>
@@ -1176,7 +1212,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>63</v>
       </c>
@@ -1189,8 +1225,11 @@
       <c r="E25" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>64</v>
       </c>
@@ -1202,6 +1241,9 @@
       </c>
       <c r="E26" s="7" t="s">
         <v>7</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criada rota de pesquisa dos temas
</commit_message>
<xml_diff>
--- a/docs/Requisitos_Funcionais.xlsx
+++ b/docs/Requisitos_Funcionais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desenvolvimento\Desktop\FORUM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE91E58-78FF-46D6-A4A7-41CCB2F2B98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5138EC-14EC-4329-A8B2-E6242CC4B48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40153BD5-6B4E-464B-9827-E0D7A3498535}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
   <si>
     <t>Tela de cadastro</t>
   </si>
@@ -540,6 +540,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -548,9 +551,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,7 +869,7 @@
   <dimension ref="B1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,12 +881,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
@@ -968,7 +968,7 @@
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -985,7 +985,7 @@
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
       <c r="E10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1019,7 +1019,7 @@
       <c r="E11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
       <c r="E12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       <c r="E16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       <c r="E17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       <c r="E18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
       <c r="E19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1159,6 +1159,9 @@
       <c r="E20" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="F20" s="15" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
@@ -1225,7 +1228,7 @@
       <c r="E25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1242,7 +1245,7 @@
       <c r="E26" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="15" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Iniciado desenvolvimento da barra de pesquisa no Frontend
</commit_message>
<xml_diff>
--- a/docs/Requisitos_Funcionais.xlsx
+++ b/docs/Requisitos_Funcionais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desenvolvimento\Desktop\FORUM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5138EC-14EC-4329-A8B2-E6242CC4B48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6883731-48D6-4817-A673-BB4E9E6F1355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40153BD5-6B4E-464B-9827-E0D7A3498535}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>Tela de cadastro</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -551,6 +554,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,7 +875,7 @@
   <dimension ref="B1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,9 +917,6 @@
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
-      <c r="F4" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -928,6 +931,9 @@
       <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="F5" s="19" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -986,7 +992,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1063,6 +1069,9 @@
       <c r="E14" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="F14" s="15" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
@@ -1077,6 +1086,9 @@
       <c r="E15" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="F15" s="15" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
@@ -1108,9 +1120,7 @@
       <c r="E17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>70</v>
-      </c>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
@@ -1125,9 +1135,7 @@
       <c r="E18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>70</v>
-      </c>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
@@ -1143,7 +1151,7 @@
         <v>7</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1175,6 +1183,9 @@
       </c>
       <c r="E21" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>